<commit_message>
added graphs based on signal song/affiliation
</commit_message>
<xml_diff>
--- a/QP-ranking.xlsx
+++ b/QP-ranking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/riuflare/Documents/GitHub/Queendom-Puzzle-Rankings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A38599E-7B4D-E946-B0C6-9A6FF0B8B354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B40FD6E-F2F4-284E-930A-4C6F5BE95D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27320" windowHeight="13340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="55">
   <si>
     <t>Nana</t>
   </si>
@@ -113,6 +113,78 @@
   </si>
   <si>
     <t>Haein</t>
+  </si>
+  <si>
+    <t>PICK on the top</t>
+  </si>
+  <si>
+    <t>PICK-CAT</t>
+  </si>
+  <si>
+    <t>Athena</t>
+  </si>
+  <si>
+    <t>DROP The Beat</t>
+  </si>
+  <si>
+    <t>SignalSong</t>
+  </si>
+  <si>
+    <t>Woo!ah!</t>
+  </si>
+  <si>
+    <t>WJSN</t>
+  </si>
+  <si>
+    <t>H1-KEY</t>
+  </si>
+  <si>
+    <t>Lovelyz</t>
+  </si>
+  <si>
+    <t>CLC</t>
+  </si>
+  <si>
+    <t>Weeekly</t>
+  </si>
+  <si>
+    <t>Purple Kiss</t>
+  </si>
+  <si>
+    <t>Cherry Bullet</t>
+  </si>
+  <si>
+    <t>Rocket Punch</t>
+  </si>
+  <si>
+    <t>TripleS</t>
+  </si>
+  <si>
+    <t>AOA</t>
+  </si>
+  <si>
+    <t>NMB48</t>
+  </si>
+  <si>
+    <t>Weki Meki</t>
+  </si>
+  <si>
+    <t>BNK48</t>
+  </si>
+  <si>
+    <t>LIGHTSUM</t>
+  </si>
+  <si>
+    <t>MOMOLAND</t>
+  </si>
+  <si>
+    <t>IZ*ONE</t>
+  </si>
+  <si>
+    <t>LABOUM</t>
+  </si>
+  <si>
+    <t>InitialGroup</t>
   </si>
 </sst>
 </file>
@@ -383,10 +455,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F141"/>
+  <dimension ref="A1:F146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -401,8 +473,12 @@
       <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -415,8 +491,12 @@
       <c r="C2" s="1">
         <v>22</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -429,8 +509,12 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -443,8 +527,12 @@
       <c r="C4" s="1">
         <v>22</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -457,8 +545,12 @@
       <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -471,8 +563,12 @@
       <c r="C6" s="1">
         <v>8</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -485,8 +581,12 @@
       <c r="C7" s="1">
         <v>8</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -499,8 +599,12 @@
       <c r="C8" s="1">
         <v>8</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -513,8 +617,12 @@
       <c r="C9" s="1">
         <v>15</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -527,8 +635,12 @@
       <c r="C10" s="1">
         <v>15</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -541,8 +653,12 @@
       <c r="C11" s="1">
         <v>15</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -555,8 +671,12 @@
       <c r="C12" s="1">
         <v>15</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -569,8 +689,12 @@
       <c r="C13" s="1">
         <v>15</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -583,8 +707,12 @@
       <c r="C14" s="1">
         <v>22</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -597,8 +725,12 @@
       <c r="C15" s="1">
         <v>8</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -611,8 +743,12 @@
       <c r="C16" s="2">
         <v>22</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -625,8 +761,12 @@
       <c r="C17" s="1">
         <v>15</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -639,8 +779,12 @@
       <c r="C18" s="1">
         <v>1</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -653,8 +797,12 @@
       <c r="C19" s="2">
         <v>22</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -667,8 +815,12 @@
       <c r="C20" s="2">
         <v>22</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -681,8 +833,12 @@
       <c r="C21" s="2">
         <v>22</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -695,8 +851,12 @@
       <c r="C22" s="1">
         <v>8</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -709,8 +869,12 @@
       <c r="C23" s="2">
         <v>22</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -723,8 +887,12 @@
       <c r="C24" s="1">
         <v>8</v>
       </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -737,8 +905,12 @@
       <c r="C25" s="1">
         <v>15</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -751,8 +923,12 @@
       <c r="C26" s="1">
         <v>1</v>
       </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -765,8 +941,12 @@
       <c r="C27" s="1">
         <v>15</v>
       </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -779,8 +959,12 @@
       <c r="C28" s="1">
         <v>1</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -793,8 +977,12 @@
       <c r="C29" s="1">
         <v>8</v>
       </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -807,8 +995,12 @@
       <c r="C30" s="1">
         <v>6</v>
       </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -821,8 +1013,12 @@
       <c r="C31" s="1">
         <v>2</v>
       </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -835,8 +1031,12 @@
       <c r="C32" s="1">
         <v>4</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -849,8 +1049,12 @@
       <c r="C33" s="1">
         <v>8</v>
       </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -863,8 +1067,12 @@
       <c r="C34" s="1">
         <v>6</v>
       </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -877,8 +1085,12 @@
       <c r="C35" s="1">
         <v>9</v>
       </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
+      <c r="D35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -891,8 +1103,12 @@
       <c r="C36" s="1">
         <v>12</v>
       </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
+      <c r="D36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -905,8 +1121,12 @@
       <c r="C37" s="1">
         <v>1</v>
       </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -919,8 +1139,12 @@
       <c r="C38" s="1">
         <v>2</v>
       </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -933,8 +1157,12 @@
       <c r="C39" s="1">
         <v>20</v>
       </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
+      <c r="D39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -947,8 +1175,12 @@
       <c r="C40" s="1">
         <v>15</v>
       </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -961,8 +1193,12 @@
       <c r="C41" s="1">
         <v>15</v>
       </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -975,8 +1211,12 @@
       <c r="C42" s="1">
         <v>24</v>
       </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -989,8 +1229,12 @@
       <c r="C43" s="1">
         <v>10</v>
       </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+      <c r="D43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1003,8 +1247,12 @@
       <c r="C44" s="1">
         <v>19</v>
       </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
+      <c r="D44" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1017,8 +1265,12 @@
       <c r="C45" s="1">
         <v>20</v>
       </c>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
+      <c r="D45" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1031,8 +1283,12 @@
       <c r="C46" s="1">
         <v>17</v>
       </c>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="D46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1045,8 +1301,12 @@
       <c r="C47" s="1">
         <v>23</v>
       </c>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
+      <c r="D47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1059,8 +1319,12 @@
       <c r="C48" s="1">
         <v>24</v>
       </c>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
+      <c r="D48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1073,8 +1337,12 @@
       <c r="C49" s="1">
         <v>10</v>
       </c>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F49" s="1"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1087,8 +1355,12 @@
       <c r="C50" s="1">
         <v>12</v>
       </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F50" s="1"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1101,8 +1373,12 @@
       <c r="C51" s="1">
         <v>17</v>
       </c>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
+      <c r="D51" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1115,8 +1391,12 @@
       <c r="C52" s="1">
         <v>12</v>
       </c>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
+      <c r="D52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1129,8 +1409,12 @@
       <c r="C53" s="1">
         <v>27</v>
       </c>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F53" s="1"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1143,8 +1427,12 @@
       <c r="C54" s="1">
         <v>22</v>
       </c>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
+      <c r="D54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1157,8 +1445,12 @@
       <c r="C55" s="1">
         <v>24</v>
       </c>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
+      <c r="D55" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1171,8 +1463,12 @@
       <c r="C56" s="1">
         <v>5</v>
       </c>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
+      <c r="D56" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1185,8 +1481,12 @@
       <c r="C57" s="2">
         <v>23</v>
       </c>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
+      <c r="D57" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1199,8 +1499,12 @@
       <c r="C58" s="1">
         <v>27</v>
       </c>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
+      <c r="D58" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1213,8 +1517,12 @@
       <c r="C59" s="2">
         <v>27</v>
       </c>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
+      <c r="D59" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="F59" s="1"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1227,8 +1535,12 @@
       <c r="C60" s="1">
         <v>1</v>
       </c>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
+      <c r="D60" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1241,8 +1553,12 @@
       <c r="C61" s="1">
         <v>2</v>
       </c>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
+      <c r="D61" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1255,8 +1571,12 @@
       <c r="C62" s="1">
         <v>3</v>
       </c>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
+      <c r="D62" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1269,8 +1589,12 @@
       <c r="C63" s="1">
         <v>4</v>
       </c>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
+      <c r="D63" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1283,8 +1607,12 @@
       <c r="C64" s="1">
         <v>5</v>
       </c>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
+      <c r="D64" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1297,8 +1625,12 @@
       <c r="C65" s="1">
         <v>6</v>
       </c>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
+      <c r="D65" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="F65" s="1"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1311,8 +1643,12 @@
       <c r="C66" s="1">
         <v>7</v>
       </c>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
+      <c r="D66" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="F66" s="1"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1325,8 +1661,12 @@
       <c r="C67" s="1">
         <v>8</v>
       </c>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
+      <c r="D67" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="1">
@@ -1338,8 +1678,12 @@
       <c r="C68" s="1">
         <v>9</v>
       </c>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
+      <c r="D68" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="1">
@@ -1351,8 +1695,12 @@
       <c r="C69" s="1">
         <v>10</v>
       </c>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
+      <c r="D69" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1365,8 +1713,12 @@
       <c r="C70" s="1">
         <v>11</v>
       </c>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
+      <c r="D70" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="F70" s="1"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1379,8 +1731,12 @@
       <c r="C71" s="1">
         <v>12</v>
       </c>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
+      <c r="D71" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="F71" s="1"/>
     </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1393,8 +1749,12 @@
       <c r="C72" s="1">
         <v>13</v>
       </c>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
+      <c r="D72" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1407,8 +1767,12 @@
       <c r="C73" s="1">
         <v>14</v>
       </c>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
+      <c r="D73" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="1">
@@ -1420,8 +1784,12 @@
       <c r="C74" s="1">
         <v>15</v>
       </c>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
+      <c r="D74" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="1">
@@ -1433,8 +1801,12 @@
       <c r="C75" s="1">
         <v>16</v>
       </c>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
+      <c r="D75" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="F75" s="1"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1447,8 +1819,12 @@
       <c r="C76" s="1">
         <v>17</v>
       </c>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
+      <c r="D76" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="F76" s="1"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1461,8 +1837,12 @@
       <c r="C77" s="1">
         <v>18</v>
       </c>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
+      <c r="D77" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="1">
@@ -1474,8 +1854,12 @@
       <c r="C78" s="1">
         <v>19</v>
       </c>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
+      <c r="D78" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F78" s="1"/>
     </row>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1488,8 +1872,12 @@
       <c r="C79" s="1">
         <v>20</v>
       </c>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
+      <c r="D79" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="1">
@@ -1501,10 +1889,14 @@
       <c r="C80" s="1">
         <v>21</v>
       </c>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-    </row>
-    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D80" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="1">
         <v>7</v>
       </c>
@@ -1514,8 +1906,14 @@
       <c r="C81" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D81" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="1">
         <v>7</v>
       </c>
@@ -1525,8 +1923,14 @@
       <c r="C82" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D82" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="1">
         <v>7</v>
       </c>
@@ -1536,8 +1940,14 @@
       <c r="C83" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D83" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="1">
         <v>7</v>
       </c>
@@ -1547,8 +1957,14 @@
       <c r="C84" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D84" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="1">
         <v>7</v>
       </c>
@@ -1558,8 +1974,14 @@
       <c r="C85" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D85" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="1">
         <v>8</v>
       </c>
@@ -1569,8 +1991,14 @@
       <c r="C86" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D86" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="1">
         <v>8</v>
       </c>
@@ -1580,8 +2008,14 @@
       <c r="C87" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D87" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="1">
         <v>8</v>
       </c>
@@ -1591,8 +2025,14 @@
       <c r="C88" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D88" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="1">
         <v>8</v>
       </c>
@@ -1602,8 +2042,14 @@
       <c r="C89" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D89" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="1">
         <v>8</v>
       </c>
@@ -1613,8 +2059,14 @@
       <c r="C90" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D90" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="1">
         <v>8</v>
       </c>
@@ -1624,8 +2076,14 @@
       <c r="C91" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D91" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="1">
         <v>8</v>
       </c>
@@ -1635,8 +2093,14 @@
       <c r="C92" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D92" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="1">
         <v>8</v>
       </c>
@@ -1646,8 +2110,14 @@
       <c r="C93" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D93" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="1">
         <v>8</v>
       </c>
@@ -1657,8 +2127,14 @@
       <c r="C94" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D94" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="1">
         <v>8</v>
       </c>
@@ -1668,8 +2144,14 @@
       <c r="C95" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D95" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="1">
         <v>8</v>
       </c>
@@ -1679,8 +2161,14 @@
       <c r="C96" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D96" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="1">
         <v>8</v>
       </c>
@@ -1690,8 +2178,14 @@
       <c r="C97" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D97" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="1">
         <v>8</v>
       </c>
@@ -1701,8 +2195,14 @@
       <c r="C98" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D98" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="1">
         <v>8</v>
       </c>
@@ -1712,8 +2212,14 @@
       <c r="C99" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D99" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="1">
         <v>8</v>
       </c>
@@ -1723,8 +2229,14 @@
       <c r="C100" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D100" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="1">
         <v>8</v>
       </c>
@@ -1734,8 +2246,14 @@
       <c r="C101" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D101" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="1">
         <v>8</v>
       </c>
@@ -1745,8 +2263,14 @@
       <c r="C102" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D102" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="1">
         <v>8</v>
       </c>
@@ -1756,8 +2280,14 @@
       <c r="C103" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D103" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="1">
         <v>8</v>
       </c>
@@ -1767,8 +2297,14 @@
       <c r="C104" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D104" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105" s="1">
         <v>8</v>
       </c>
@@ -1778,8 +2314,14 @@
       <c r="C105" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D105" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106" s="1">
         <v>8</v>
       </c>
@@ -1789,8 +2331,14 @@
       <c r="C106" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D106" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="1">
         <v>9</v>
       </c>
@@ -1800,8 +2348,14 @@
       <c r="C107" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D107" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A108" s="1">
         <v>9</v>
       </c>
@@ -1811,8 +2365,14 @@
       <c r="C108" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D108" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="1">
         <v>9</v>
       </c>
@@ -1822,8 +2382,14 @@
       <c r="C109" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D109" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="1">
         <v>9</v>
       </c>
@@ -1833,8 +2399,14 @@
       <c r="C110" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D110" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="1">
         <v>9</v>
       </c>
@@ -1844,8 +2416,14 @@
       <c r="C111" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D111" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A112" s="1">
         <v>9</v>
       </c>
@@ -1855,8 +2433,14 @@
       <c r="C112" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D112" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="1">
         <v>9</v>
       </c>
@@ -1866,8 +2450,14 @@
       <c r="C113" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D113" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="1">
         <v>9</v>
       </c>
@@ -1877,8 +2467,14 @@
       <c r="C114" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D114" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="1">
         <v>9</v>
       </c>
@@ -1888,8 +2484,14 @@
       <c r="C115" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D115" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116" s="1">
         <v>9</v>
       </c>
@@ -1899,8 +2501,14 @@
       <c r="C116" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D116" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A117" s="1">
         <v>9</v>
       </c>
@@ -1910,8 +2518,14 @@
       <c r="C117" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D117" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A118" s="1">
         <v>9</v>
       </c>
@@ -1921,8 +2535,14 @@
       <c r="C118" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D118" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A119" s="1">
         <v>9</v>
       </c>
@@ -1932,8 +2552,14 @@
       <c r="C119" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D119" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120" s="1">
         <v>9</v>
       </c>
@@ -1943,8 +2569,14 @@
       <c r="C120" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D120" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A121" s="1">
         <v>9</v>
       </c>
@@ -1954,8 +2586,14 @@
       <c r="C121" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D121" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A122" s="1">
         <v>9</v>
       </c>
@@ -1965,8 +2603,14 @@
       <c r="C122" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D122" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A123" s="1">
         <v>9</v>
       </c>
@@ -1976,8 +2620,14 @@
       <c r="C123" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D123" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A124" s="1">
         <v>9</v>
       </c>
@@ -1987,8 +2637,14 @@
       <c r="C124" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D124" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A125" s="1">
         <v>9</v>
       </c>
@@ -1998,8 +2654,14 @@
       <c r="C125" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D125" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A126" s="1">
         <v>9</v>
       </c>
@@ -2009,8 +2671,14 @@
       <c r="C126" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D126" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A127" s="1">
         <v>9</v>
       </c>
@@ -2020,8 +2688,14 @@
       <c r="C127" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D127" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A128" s="1">
         <v>10</v>
       </c>
@@ -2031,8 +2705,14 @@
       <c r="C128" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D128" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A129" s="1">
         <v>10</v>
       </c>
@@ -2042,8 +2722,14 @@
       <c r="C129" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D129" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A130" s="1">
         <v>10</v>
       </c>
@@ -2053,8 +2739,14 @@
       <c r="C130" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D130" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131" s="1">
         <v>10</v>
       </c>
@@ -2064,8 +2756,14 @@
       <c r="C131" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D131" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A132" s="1">
         <v>10</v>
       </c>
@@ -2075,8 +2773,14 @@
       <c r="C132" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D132" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A133" s="1">
         <v>10</v>
       </c>
@@ -2086,8 +2790,14 @@
       <c r="C133" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D133" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A134" s="1">
         <v>10</v>
       </c>
@@ -2097,8 +2807,14 @@
       <c r="C134" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D134" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A135" s="1">
         <v>10</v>
       </c>
@@ -2108,8 +2824,14 @@
       <c r="C135" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D135" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136" s="1">
         <v>10</v>
       </c>
@@ -2119,8 +2841,14 @@
       <c r="C136" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D136" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A137" s="1">
         <v>10</v>
       </c>
@@ -2130,8 +2858,14 @@
       <c r="C137" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D137" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A138" s="1">
         <v>10</v>
       </c>
@@ -2141,8 +2875,14 @@
       <c r="C138" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D138" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A139" s="1">
         <v>10</v>
       </c>
@@ -2152,8 +2892,14 @@
       <c r="C139" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D139" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A140" s="1">
         <v>10</v>
       </c>
@@ -2163,8 +2909,14 @@
       <c r="C140" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D140" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A141" s="1">
         <v>10</v>
       </c>
@@ -2174,6 +2926,27 @@
       <c r="C141" s="1">
         <v>11</v>
       </c>
+      <c r="D141" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E142" s="2"/>
+    </row>
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E143" s="2"/>
+    </row>
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E144" s="2"/>
+    </row>
+    <row r="145" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E145" s="2"/>
+    </row>
+    <row r="146" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E146" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>